<commit_message>
data input and add to S1 analysis
</commit_message>
<xml_diff>
--- a/S2 - No-dig broccoli/data.xlsx
+++ b/S2 - No-dig broccoli/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\My Drive\Play\Gardening\ebg\ebg_repo\S2 - No-dig broccoli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2169A7-3FA9-49E9-BABA-CBD86CEFC34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6C25A1-20A2-4E23-BE67-0BDD0EFBFF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
   <si>
     <t>height_30d_mm</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>bed_type</t>
+  </si>
+  <si>
+    <t>yield_g</t>
+  </si>
+  <si>
+    <t>harvest_date</t>
   </si>
 </sst>
 </file>
@@ -382,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,9 +399,10 @@
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -414,8 +421,14 @@
       <c r="F1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -432,7 +445,7 @@
         <v>45407</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -449,7 +462,7 @@
         <v>45407</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -466,7 +479,7 @@
         <v>45407</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -483,7 +496,7 @@
         <v>45407</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -500,7 +513,7 @@
         <v>45407</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -517,7 +530,7 @@
         <v>45407</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -534,7 +547,7 @@
         <v>45407</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -551,7 +564,7 @@
         <v>45407</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -568,7 +581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -585,7 +598,7 @@
         <v>45407</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -602,7 +615,7 @@
         <v>45407</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -619,7 +632,7 @@
         <v>45407</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -635,8 +648,17 @@
       <c r="E14" s="1">
         <v>45407</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>327.10000000000002</v>
+      </c>
+      <c r="H14" s="1">
+        <v>45520</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>

</xml_diff>